<commit_message>
Make changes from NOAA comments
</commit_message>
<xml_diff>
--- a/CODE/Data/Dc_cmax20-b250_D075_J100_A050_Sm025_nmort1_BE075_noCC_RE00100_Ka050/LHS_param6_mid6_samek_bestAIC_params_Fupneg_mult8_Pneg2_mult3.xlsx
+++ b/CODE/Data/Dc_cmax20-b250_D075_J100_A050_Sm025_nmort1_BE075_noCC_RE00100_Ka050/LHS_param6_mid6_samek_bestAIC_params_Fupneg_mult8_Pneg2_mult3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpetrik/Dropbox/Princeton/FEISTY/CODE/Data/Dc_cmax20-b250_D075_J100_A050_Sm025_nmort1_BE075_noCC_RE00100_Ka050/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB96C2A5-9C7D-B445-9C16-46952E17A876}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E842B0-0704-E94E-BDD0-BE1A5038C1CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="960" windowWidth="26940" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>ParamSet</t>
   </si>
@@ -663,13 +663,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1028,7 +1034,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:G34"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1833,7 +1839,7 @@
         <v>0.60091404761740896</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1852,8 +1858,11 @@
       <c r="G19" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>0.6</v>
       </c>
@@ -1874,8 +1883,11 @@
       <c r="G20" s="3">
         <v>6.3E-2</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="4">
+        <v>583.36161269206798</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>0.75</v>
       </c>
@@ -1896,8 +1908,11 @@
       <c r="G21" s="3">
         <v>9.5500000000000002E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="4">
+        <v>583.38003501001504</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>0.6</v>
       </c>
@@ -1918,8 +1933,11 @@
       <c r="G22" s="3">
         <v>7.9250000000000001E-2</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H22" s="4">
+        <v>586.73392079839596</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>0.75</v>
       </c>
@@ -1940,8 +1958,11 @@
       <c r="G23" s="3">
         <v>7.9250000000000001E-2</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H23" s="4">
+        <v>592.906166900215</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>0.6</v>
       </c>
@@ -1962,8 +1983,11 @@
       <c r="G24" s="3">
         <v>9.5500000000000002E-2</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H24" s="4">
+        <v>593.33064933845299</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="2">
         <v>0.75</v>
       </c>
@@ -1984,8 +2008,11 @@
       <c r="G25" s="3">
         <v>6.3E-2</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H25" s="4">
+        <v>602.47654986790599</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" s="2">
         <v>0.6</v>
       </c>
@@ -2006,8 +2033,11 @@
       <c r="G26" s="3">
         <v>7.9250000000000001E-2</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H26" s="4">
+        <v>622.97859569073205</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" s="2">
         <v>0.6</v>
       </c>
@@ -2028,8 +2058,11 @@
       <c r="G27" s="3">
         <v>6.3E-2</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H27" s="4">
+        <v>625.30742618901297</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="2">
         <v>0.6</v>
       </c>
@@ -2050,8 +2083,11 @@
       <c r="G28" s="3">
         <v>7.9250000000000001E-2</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H28" s="4">
+        <v>628.889625459228</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" s="2">
         <v>0.6</v>
       </c>
@@ -2072,8 +2108,11 @@
       <c r="G29" s="3">
         <v>6.3E-2</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H29" s="4">
+        <v>629.60981328427999</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" s="2">
         <v>0.6</v>
       </c>
@@ -2094,8 +2133,11 @@
       <c r="G30" s="3">
         <v>9.5500000000000002E-2</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H30" s="4">
+        <v>632.83683092553201</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="2">
         <v>0.75</v>
       </c>
@@ -2116,8 +2158,11 @@
       <c r="G31" s="3">
         <v>9.5500000000000002E-2</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H31" s="4">
+        <v>636.98660626384901</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="2">
         <v>0.6</v>
       </c>
@@ -2138,8 +2183,11 @@
       <c r="G32" s="3">
         <v>9.5500000000000002E-2</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H32" s="4">
+        <v>638.869053592471</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" s="2">
         <v>0.75</v>
       </c>
@@ -2160,8 +2208,11 @@
       <c r="G33" s="3">
         <v>7.9250000000000001E-2</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H33" s="4">
+        <v>639.85211856129104</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" s="2">
         <v>0.67500000000000004</v>
       </c>
@@ -2181,6 +2232,9 @@
       </c>
       <c r="G34" s="3">
         <v>7.9250000000000001E-2</v>
+      </c>
+      <c r="H34" s="4">
+        <v>642.63229332590799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>